<commit_message>
güncel veri temizleme dosyası
</commit_message>
<xml_diff>
--- a/Foodfacts/kume_verisi.xlsx
+++ b/Foodfacts/kume_verisi.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeyne\QueensOfData\Foodfacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0CF6A7-D0A1-4BC5-8417-857AD497DCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01ABB88-A004-4716-A3F8-EEB70CB8B390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="104">
   <si>
     <t>MyColumn</t>
   </si>
@@ -352,7 +365,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +387,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -413,6 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,514 +735,788 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="66.453125" customWidth="1"/>
-    <col min="6" max="6" width="23.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D2" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="D9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="D10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="D13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="D14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="D15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="D16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D17" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D19" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D20" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D21" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D22" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D23" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D24" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D25" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D26" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D27" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D28" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D29" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D30" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D31" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D32" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D33" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D34" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D35" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D36" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D37" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D38" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D39" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D40" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D41" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D42" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D43" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D44" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D45" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D46" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D47" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D48" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D49" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D50" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D51" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D52" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D53" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D54" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D55" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D56" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D57" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D58" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D59" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D60" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D61" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D62" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D63" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D64" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D65" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D66" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D67" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D68" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D69" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D70" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D71" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D72" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D73" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D74" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D75" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D76" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D77" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D78" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D79" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D80" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D81" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D82" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D83" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D84" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D85" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D86" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D87" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D88" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D89" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="D90" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>90</v>
       </c>
+      <c r="D91" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D93" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>